<commit_message>
Create the Excel test file for Vission and mission
</commit_message>
<xml_diff>
--- a/Utilities/VisionandMission.xlsx
+++ b/Utilities/VisionandMission.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Desktop\SmartCliff-Admin\Utilities\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED6EB03D-2B7D-47B2-9465-3BE21104D962}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E2DDE14-20B4-4003-9CA3-2172B08820C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{E81C43CD-FD33-42AF-B732-FD19A9EFAFEA}"/>
   </bookViews>
@@ -34,22 +34,38 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>Welcome to the smartcliff</t>
   </si>
   <si>
     <t>${descriptiontext}</t>
   </si>
+  <si>
+    <t>Welcome to the Kiot</t>
+  </si>
+  <si>
+    <t>Batman</t>
+  </si>
+  <si>
+    <t>IronMan</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -75,9 +91,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -394,37 +416,47 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C0DF830-EB65-4864-AADE-C8E1A0F6BF72}">
-  <dimension ref="A1:A5"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="40.33203125" customWidth="1"/>
+    <col min="2" max="2" width="18" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="50.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" ht="50.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="1"/>
+    </row>
+    <row r="3" spans="1:4" ht="39" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="2"/>
+    </row>
+    <row r="4" spans="1:4" ht="43.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:1" ht="39" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="1"/>
-    </row>
-    <row r="4" spans="1:1" ht="43.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="1"/>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A5" s="1"/>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
+        <v>4</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add the tags for all tests
</commit_message>
<xml_diff>
--- a/Utilities/VisionandMission.xlsx
+++ b/Utilities/VisionandMission.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Desktop\SmartCliff-Admin\Utilities\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E2DDE14-20B4-4003-9CA3-2172B08820C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65A44EC5-986F-490B-8983-D71739983BB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{E81C43CD-FD33-42AF-B732-FD19A9EFAFEA}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Welcome to the smartcliff</t>
   </si>
@@ -49,6 +49,9 @@
   </si>
   <si>
     <t>IronMan</t>
+  </si>
+  <si>
+    <t>Hulk</t>
   </si>
 </sst>
 </file>
@@ -416,15 +419,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C0DF830-EB65-4864-AADE-C8E1A0F6BF72}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="40.33203125" customWidth="1"/>
+    <col min="1" max="1" width="42.21875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -435,25 +438,33 @@
     </row>
     <row r="2" spans="1:4" ht="50.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B2" s="1"/>
     </row>
     <row r="3" spans="1:4" ht="39" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D3" s="2"/>
     </row>
     <row r="4" spans="1:4" ht="43.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="37.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="3" t="s">
+    <row r="6" spans="1:4" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="3" t="s">
         <v>4</v>
       </c>
+    </row>
+    <row r="7" spans="1:4" ht="54.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
completed the Vission and Mission feature
</commit_message>
<xml_diff>
--- a/Utilities/VisionandMission.xlsx
+++ b/Utilities/VisionandMission.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Desktop\SmartCliff-Admin\Utilities\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65A44EC5-986F-490B-8983-D71739983BB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C466C00-2A03-451D-A887-B33916208AEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{E81C43CD-FD33-42AF-B732-FD19A9EFAFEA}"/>
   </bookViews>
@@ -422,7 +422,7 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>